<commit_message>
he actualizado el back log
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -206,13 +206,22 @@
     <t>Como inspector/comisario quiero botones y switches en el dashboard de sensores para controlar luces LEDs y puertas para actuar sobre las instalaciones</t>
   </si>
   <si>
-    <t>Modificacion de la vista de sensores y añadir controles</t>
+    <t>Implementar Control de  Permisos</t>
+  </si>
+  <si>
+    <t>Implementar Controles de Panel Derecho</t>
+  </si>
+  <si>
+    <t>Implementar Controles del Mapa</t>
   </si>
   <si>
     <t>Como desarrollador quiero que el controlador mueste/oculte los controles y conecte sus eventos para asegurar que el policia no pueda controlar actuadores</t>
   </si>
   <si>
-    <t>Creacion de la logica de permisos en los actuadores</t>
+    <t>Implementar Controles de Actuadores</t>
+  </si>
+  <si>
+    <t>Conectar Vista y Controlador</t>
   </si>
   <si>
     <t>CUARTO SPRINT</t>
@@ -221,19 +230,65 @@
     <t>Como comisario quiero funciones en el modelo para gestionar la lista de usuarios para administar las cuentas del sistema</t>
   </si>
   <si>
-    <t>Creacion del modelo de usuarios CRUD</t>
+    <t>Implementar Funciones de Usuarios</t>
   </si>
   <si>
     <t>Como comisario quiero una interfaz para añadir, editar y borrar usuarios para administar las cuentas del sistema</t>
   </si>
   <si>
-    <t>Creacion de la vista de gestion de usuarios CRUD</t>
+    <t>Diseñar Vista de Usuarios</t>
   </si>
   <si>
     <t>Como desarrollador quiero que la vista de gestion de usuarios solo sea accesible para el comisario para cumplir con los requisitos de seguridad</t>
   </si>
   <si>
-    <t>Creacion de la logica de permisos en el controlador de ususarios</t>
+    <t>Implementar Controlador de Usuarios</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Trebuchet MS"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Como desarrollador quiero un archivo </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Trebuchet MS"/>
+        <color rgb="FF1155CC"/>
+        <sz val="12.0"/>
+        <u/>
+      </rPr>
+      <t>READ.md</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Trebuchet MS"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> completo y el codigo limpio para facilitar la instalacion y la correccion del proyecto</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Trebuchet MS"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Redactar </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Trebuchet MS"/>
+        <color rgb="FF1155CC"/>
+        <sz val="12.0"/>
+        <u/>
+      </rPr>
+      <t>READ.md</t>
+    </r>
+  </si>
+  <si>
+    <t>Verificacion Final</t>
   </si>
   <si>
     <t>TIPOS DE PRIORIDAD</t>
@@ -263,7 +318,7 @@
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="dd&quot;/&quot;mm&quot;/&quot;yy"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -407,6 +462,18 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <color rgb="FFFBBC05"/>
       <name val="Roboto"/>
@@ -460,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="65">
+  <borders count="60">
     <border/>
     <border>
       <left/>
@@ -817,18 +884,8 @@
       </top>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <top/>
       <bottom/>
     </border>
     <border>
@@ -836,25 +893,21 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top/>
-    </border>
-    <border>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <right/>
@@ -864,31 +917,25 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -911,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="181">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1201,121 +1248,144 @@
     <xf borderId="39" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="52" fillId="2" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="53" fillId="2" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="54" fillId="2" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="55" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="21" fillId="2" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="2" fontId="22" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="24" fillId="2" fontId="22" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="52" fillId="2" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="53" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="23" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="23" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="23" fillId="2" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="54" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="22" fillId="2" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="56" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="55" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="39" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="55" fillId="2" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="42" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="42" fillId="5" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="42" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="42" fillId="5" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="45" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="39" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="39" fillId="2" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="48" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="2" fontId="22" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="20" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="21" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="42" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="21" fillId="2" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="56" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="21" fillId="2" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="21" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="56" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="53" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="57" fillId="2" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="23" fillId="2" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="23" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="24" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="37" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="37" fillId="2" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="38" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="36" fillId="2" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="57" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="46" fillId="2" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf borderId="58" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="59" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="2" fontId="22" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="26" fillId="2" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="26" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="27" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="28" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="29" fillId="2" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="22" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="41" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="60" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="25" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="26" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="26" fillId="5" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="26" fillId="5" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="26" fillId="5" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="30" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="61" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="62" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="62" fillId="5" fontId="24" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="62" fillId="5" fontId="23" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="62" fillId="5" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="63" fillId="5" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1329,34 +1399,35 @@
     <xf borderId="11" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="2" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="64" fillId="5" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="59" fillId="5" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="26" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="2" fontId="26" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="27" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="2" fontId="29" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="64" fillId="5" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="59" fillId="5" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="30" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="2" fontId="32" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2304,74 +2375,80 @@
     </row>
     <row r="34" ht="24.75" customHeight="1">
       <c r="A34" s="109"/>
-      <c r="B34" s="117" t="s">
+      <c r="B34" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="118"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="118"/>
-      <c r="G34" s="118"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="118"/>
-      <c r="J34" s="118"/>
-      <c r="K34" s="118"/>
-      <c r="L34" s="119"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="118">
+        <v>0.0</v>
+      </c>
+      <c r="K34" s="119">
+        <v>0.0</v>
+      </c>
+      <c r="L34" s="120">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="35" ht="61.5" customHeight="1">
-      <c r="A35" s="120"/>
-      <c r="B35" s="121" t="s">
+      <c r="A35" s="121"/>
+      <c r="B35" s="122" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="122" t="s">
+      <c r="C35" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="123"/>
-      <c r="E35" s="123"/>
-      <c r="F35" s="124">
+      <c r="D35" s="124"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="125">
         <v>3.0</v>
       </c>
-      <c r="G35" s="122"/>
-      <c r="H35" s="125" t="s">
+      <c r="G35" s="123"/>
+      <c r="H35" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="I35" s="125" t="s">
+      <c r="I35" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="J35" s="126">
+      <c r="J35" s="127">
         <v>0.0</v>
       </c>
-      <c r="K35" s="122">
+      <c r="K35" s="123">
         <v>0.0</v>
       </c>
-      <c r="L35" s="127">
+      <c r="L35" s="128">
         <v>0.0</v>
       </c>
     </row>
     <row r="36" ht="61.5" customHeight="1">
-      <c r="A36" s="128"/>
-      <c r="B36" s="129" t="s">
+      <c r="A36" s="129"/>
+      <c r="B36" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="130" t="s">
+      <c r="C36" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="131"/>
-      <c r="E36" s="131"/>
-      <c r="F36" s="132">
+      <c r="D36" s="130"/>
+      <c r="E36" s="130"/>
+      <c r="F36" s="96">
         <v>3.0</v>
       </c>
-      <c r="G36" s="133"/>
-      <c r="H36" s="130" t="s">
+      <c r="G36" s="131"/>
+      <c r="H36" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="I36" s="130" t="s">
+      <c r="I36" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="126">
+      <c r="J36" s="132">
         <v>0.0</v>
       </c>
-      <c r="K36" s="125">
+      <c r="K36" s="133">
         <v>0.0</v>
       </c>
       <c r="L36" s="134">
@@ -2379,299 +2456,402 @@
       </c>
     </row>
     <row r="37" ht="61.5" customHeight="1">
-      <c r="A37" s="128"/>
-      <c r="B37" s="129" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="130" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
-      <c r="F37" s="132">
-        <v>3.0</v>
-      </c>
-      <c r="G37" s="133"/>
-      <c r="H37" s="130" t="s">
+      <c r="A37" s="129"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="135"/>
+      <c r="E37" s="135"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="I37" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="I37" s="130" t="s">
-        <v>66</v>
-      </c>
-      <c r="J37" s="126">
-        <v>0.0</v>
-      </c>
-      <c r="K37" s="125">
-        <v>0.0</v>
-      </c>
-      <c r="L37" s="134">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="38" ht="24.75" customHeight="1">
-      <c r="A38" s="47"/>
-      <c r="B38" s="135" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="136"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="67"/>
+    </row>
+    <row r="38" ht="61.5" customHeight="1">
+      <c r="A38" s="129"/>
+      <c r="B38" s="98"/>
+      <c r="C38" s="92"/>
       <c r="D38" s="136"/>
       <c r="E38" s="136"/>
-      <c r="F38" s="136"/>
-      <c r="G38" s="136"/>
-      <c r="H38" s="136"/>
-      <c r="I38" s="137"/>
-      <c r="J38" s="138">
+      <c r="F38" s="92"/>
+      <c r="G38" s="92"/>
+      <c r="H38" s="87"/>
+      <c r="I38" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="J38" s="92"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="93"/>
+    </row>
+    <row r="39" ht="61.5" customHeight="1">
+      <c r="A39" s="129"/>
+      <c r="B39" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="101" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="137"/>
+      <c r="E39" s="137"/>
+      <c r="F39" s="96">
+        <v>3.0</v>
+      </c>
+      <c r="G39" s="131"/>
+      <c r="H39" s="102" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="J39" s="138">
         <v>0.0</v>
       </c>
-      <c r="K38" s="139">
+      <c r="K39" s="82">
         <v>0.0</v>
       </c>
-      <c r="L38" s="140">
+      <c r="L39" s="83">
         <v>0.0</v>
       </c>
     </row>
-    <row r="39" ht="62.25" customHeight="1">
-      <c r="A39" s="109"/>
-      <c r="B39" s="141" t="s">
+    <row r="40" ht="61.5" customHeight="1">
+      <c r="A40" s="129"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="139"/>
+      <c r="E40" s="139"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="92"/>
+      <c r="H40" s="87"/>
+      <c r="I40" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="J40" s="92"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="93"/>
+    </row>
+    <row r="41" ht="24.75" customHeight="1">
+      <c r="A41" s="47"/>
+      <c r="B41" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="118">
+        <v>0.0</v>
+      </c>
+      <c r="K41" s="119">
+        <v>0.0</v>
+      </c>
+      <c r="L41" s="140">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42" ht="62.25" customHeight="1">
+      <c r="A42" s="109"/>
+      <c r="B42" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="142" t="s">
+      <c r="C42" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="143"/>
-      <c r="E39" s="143"/>
-      <c r="F39" s="144">
+      <c r="D42" s="143"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="144">
         <v>4.0</v>
       </c>
-      <c r="G39" s="145"/>
-      <c r="H39" s="142" t="s">
-        <v>68</v>
-      </c>
-      <c r="I39" s="142" t="s">
+      <c r="G42" s="145"/>
+      <c r="H42" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="I42" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="J42" s="146">
+        <v>0.0</v>
+      </c>
+      <c r="K42" s="147">
+        <v>0.0</v>
+      </c>
+      <c r="L42" s="148">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" ht="62.25" customHeight="1">
+      <c r="A43" s="109"/>
+      <c r="B43" s="149" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="150" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="124"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="151">
+        <v>4.0</v>
+      </c>
+      <c r="G43" s="152"/>
+      <c r="H43" s="126" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="J43" s="127">
+        <v>0.0</v>
+      </c>
+      <c r="K43" s="150">
+        <v>0.0</v>
+      </c>
+      <c r="L43" s="153">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" ht="62.25" customHeight="1">
+      <c r="A44" s="109"/>
+      <c r="B44" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="82" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="154"/>
+      <c r="E44" s="154"/>
+      <c r="F44" s="155">
+        <v>4.0</v>
+      </c>
+      <c r="G44" s="156"/>
+      <c r="H44" s="102" t="s">
+        <v>75</v>
+      </c>
+      <c r="I44" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="J44" s="157">
+        <v>0.0</v>
+      </c>
+      <c r="K44" s="102">
+        <v>0.0</v>
+      </c>
+      <c r="L44" s="158">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" ht="62.25" customHeight="1">
+      <c r="A45" s="109"/>
+      <c r="B45" s="98"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="159"/>
+      <c r="E45" s="159"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="90"/>
+      <c r="H45" s="87"/>
+      <c r="I45" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="J39" s="146">
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="160"/>
+    </row>
+    <row r="46" ht="62.25" customHeight="1">
+      <c r="A46" s="109"/>
+      <c r="B46" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="159"/>
+      <c r="E46" s="159"/>
+      <c r="F46" s="161">
+        <v>4.0</v>
+      </c>
+      <c r="G46" s="162"/>
+      <c r="H46" s="163" t="s">
+        <v>77</v>
+      </c>
+      <c r="I46" s="164" t="s">
+        <v>78</v>
+      </c>
+      <c r="J46" s="165">
         <v>0.0</v>
       </c>
-      <c r="K39" s="147">
+      <c r="K46" s="55">
         <v>0.0</v>
       </c>
-      <c r="L39" s="148">
+      <c r="L46" s="61">
         <v>0.0</v>
       </c>
     </row>
-    <row r="40" ht="62.25" customHeight="1">
-      <c r="A40" s="109"/>
-      <c r="B40" s="149" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="150" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="151"/>
-      <c r="E40" s="151"/>
-      <c r="F40" s="152">
-        <v>4.0</v>
-      </c>
-      <c r="G40" s="153"/>
-      <c r="H40" s="150" t="s">
-        <v>70</v>
-      </c>
-      <c r="I40" s="150" t="s">
-        <v>71</v>
-      </c>
-      <c r="J40" s="126">
-        <v>0.0</v>
-      </c>
-      <c r="K40" s="150">
-        <v>0.0</v>
-      </c>
-      <c r="L40" s="154">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="41" ht="62.25" customHeight="1">
-      <c r="A41" s="109"/>
-      <c r="B41" s="155" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="156" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="157"/>
-      <c r="E41" s="157"/>
-      <c r="F41" s="158">
-        <v>4.0</v>
-      </c>
-      <c r="G41" s="159"/>
-      <c r="H41" s="156" t="s">
-        <v>72</v>
-      </c>
-      <c r="I41" s="156" t="s">
-        <v>73</v>
-      </c>
-      <c r="J41" s="126">
-        <v>0.0</v>
-      </c>
-      <c r="K41" s="156">
-        <v>0.0</v>
-      </c>
-      <c r="L41" s="160">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="42" ht="18.0" customHeight="1">
-      <c r="A42" s="34"/>
-      <c r="B42" s="161"/>
-      <c r="C42" s="162"/>
-      <c r="D42" s="162"/>
-      <c r="E42" s="163"/>
-      <c r="F42" s="161"/>
-      <c r="G42" s="161"/>
-      <c r="H42" s="161"/>
-      <c r="I42" s="162"/>
-      <c r="J42" s="164"/>
-      <c r="K42" s="164"/>
-      <c r="L42" s="165"/>
-    </row>
-    <row r="43" ht="18.0" customHeight="1">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="166"/>
-      <c r="K43" s="166"/>
-      <c r="L43" s="167"/>
-    </row>
-    <row r="44" ht="30.0" customHeight="1">
-      <c r="A44" s="109"/>
-      <c r="B44" s="168" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="168" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="169"/>
-      <c r="E44" s="169"/>
-      <c r="F44" s="120"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="120"/>
-      <c r="I44" s="170"/>
-      <c r="J44" s="171"/>
-      <c r="K44" s="167"/>
-      <c r="L44" s="167"/>
-    </row>
-    <row r="45" ht="18.75" customHeight="1">
-      <c r="A45" s="109"/>
-      <c r="B45" s="172" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="172" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" s="169"/>
-      <c r="E45" s="169"/>
-      <c r="F45" s="120"/>
-      <c r="G45" s="120"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="173"/>
-      <c r="J45" s="171"/>
-      <c r="K45" s="167"/>
-      <c r="L45" s="167"/>
-    </row>
-    <row r="46" ht="19.5" customHeight="1">
-      <c r="A46" s="109"/>
-      <c r="B46" s="172" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="172" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="169"/>
-      <c r="E46" s="169"/>
-      <c r="F46" s="120"/>
-      <c r="G46" s="120"/>
-      <c r="H46" s="120"/>
-      <c r="I46" s="173"/>
-      <c r="J46" s="171"/>
-      <c r="K46" s="167"/>
-      <c r="L46" s="167"/>
-    </row>
-    <row r="47" ht="18.75" customHeight="1">
+    <row r="47" ht="62.25" customHeight="1">
       <c r="A47" s="109"/>
-      <c r="B47" s="172" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="172" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="169"/>
-      <c r="E47" s="169"/>
-      <c r="F47" s="120"/>
-      <c r="G47" s="120"/>
-      <c r="H47" s="120"/>
-      <c r="I47" s="173"/>
-      <c r="J47" s="171"/>
-      <c r="K47" s="167"/>
-      <c r="L47" s="167"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="159"/>
+      <c r="E47" s="159"/>
+      <c r="F47" s="89"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="90"/>
+      <c r="I47" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="J47" s="92"/>
+      <c r="K47" s="89"/>
+      <c r="L47" s="93"/>
     </row>
     <row r="48" ht="18.0" customHeight="1">
-      <c r="A48" s="109"/>
-      <c r="B48" s="174"/>
-      <c r="C48" s="172" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="169"/>
-      <c r="E48" s="169"/>
-      <c r="F48" s="120"/>
-      <c r="G48" s="120"/>
-      <c r="H48" s="120"/>
-      <c r="I48" s="173"/>
-      <c r="J48" s="171"/>
-      <c r="K48" s="167"/>
-      <c r="L48" s="167"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="166"/>
+      <c r="C48" s="167"/>
+      <c r="D48" s="167"/>
+      <c r="E48" s="168"/>
+      <c r="F48" s="166"/>
+      <c r="G48" s="166"/>
+      <c r="H48" s="166"/>
+      <c r="I48" s="167"/>
+      <c r="J48" s="169"/>
+      <c r="K48" s="169"/>
+      <c r="L48" s="170"/>
     </row>
     <row r="49" ht="18.0" customHeight="1">
-      <c r="A49" s="109"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="34"/>
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="35"/>
       <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
+      <c r="G49" s="35"/>
       <c r="H49" s="34"/>
       <c r="I49" s="33"/>
-      <c r="J49" s="166"/>
-      <c r="K49" s="166"/>
-      <c r="L49" s="167"/>
-    </row>
-    <row r="50" ht="18.0" customHeight="1">
+      <c r="J49" s="171"/>
+      <c r="K49" s="171"/>
+      <c r="L49" s="172"/>
+    </row>
+    <row r="50" ht="30.0" customHeight="1">
       <c r="A50" s="109"/>
-      <c r="B50" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="166"/>
-      <c r="K50" s="166"/>
-      <c r="L50" s="167"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
+      <c r="B50" s="173" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="173" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="174"/>
+      <c r="E50" s="174"/>
+      <c r="F50" s="175"/>
+      <c r="G50" s="175"/>
+      <c r="H50" s="175"/>
+      <c r="I50" s="176"/>
+      <c r="J50" s="177"/>
+      <c r="K50" s="172"/>
+      <c r="L50" s="172"/>
+    </row>
+    <row r="51" ht="18.75" customHeight="1">
+      <c r="A51" s="109"/>
+      <c r="B51" s="178" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="178" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="174"/>
+      <c r="E51" s="174"/>
+      <c r="F51" s="175"/>
+      <c r="G51" s="175"/>
+      <c r="H51" s="175"/>
+      <c r="I51" s="179"/>
+      <c r="J51" s="177"/>
+      <c r="K51" s="172"/>
+      <c r="L51" s="172"/>
+    </row>
+    <row r="52" ht="19.5" customHeight="1">
+      <c r="A52" s="109"/>
+      <c r="B52" s="178" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="178" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="174"/>
+      <c r="E52" s="174"/>
+      <c r="F52" s="175"/>
+      <c r="G52" s="175"/>
+      <c r="H52" s="175"/>
+      <c r="I52" s="179"/>
+      <c r="J52" s="177"/>
+      <c r="K52" s="172"/>
+      <c r="L52" s="172"/>
+    </row>
+    <row r="53" ht="18.75" customHeight="1">
+      <c r="A53" s="109"/>
+      <c r="B53" s="178" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="178" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="174"/>
+      <c r="E53" s="174"/>
+      <c r="F53" s="175"/>
+      <c r="G53" s="175"/>
+      <c r="H53" s="175"/>
+      <c r="I53" s="179"/>
+      <c r="J53" s="177"/>
+      <c r="K53" s="172"/>
+      <c r="L53" s="172"/>
+    </row>
+    <row r="54" ht="18.0" customHeight="1">
+      <c r="A54" s="109"/>
+      <c r="B54" s="180"/>
+      <c r="C54" s="178" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="174"/>
+      <c r="E54" s="174"/>
+      <c r="F54" s="175"/>
+      <c r="G54" s="175"/>
+      <c r="H54" s="175"/>
+      <c r="I54" s="179"/>
+      <c r="J54" s="177"/>
+      <c r="K54" s="172"/>
+      <c r="L54" s="172"/>
+    </row>
+    <row r="55" ht="18.0" customHeight="1">
+      <c r="A55" s="109"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="171"/>
+      <c r="K55" s="171"/>
+      <c r="L55" s="172"/>
+    </row>
+    <row r="56" ht="18.0" customHeight="1">
+      <c r="A56" s="109"/>
+      <c r="B56" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="171"/>
+      <c r="K56" s="171"/>
+      <c r="L56" s="172"/>
+    </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1"/>
@@ -3639,50 +3819,14 @@
     <row r="1021" ht="15.75" customHeight="1"/>
     <row r="1022" ht="15.75" customHeight="1"/>
     <row r="1023" ht="15.75" customHeight="1"/>
+    <row r="1024" ht="15.75" customHeight="1"/>
+    <row r="1025" ht="15.75" customHeight="1"/>
+    <row r="1026" ht="15.75" customHeight="1"/>
+    <row r="1027" ht="15.75" customHeight="1"/>
+    <row r="1028" ht="15.75" customHeight="1"/>
+    <row r="1029" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="H25:H27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="J30:J33"/>
-    <mergeCell ref="K30:K33"/>
-    <mergeCell ref="L30:L33"/>
+  <mergeCells count="108">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="B3:C3"/>
@@ -3717,6 +3861,80 @@
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="J30:J33"/>
+    <mergeCell ref="K30:K33"/>
+    <mergeCell ref="L30:L33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="L46:L47"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="L36:L38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="J36:J38"/>
+    <mergeCell ref="K36:K38"/>
   </mergeCells>
   <conditionalFormatting sqref="K8">
     <cfRule type="colorScale" priority="1">
@@ -3729,16 +3947,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C10 C13 C16 C18 C22 C25 C28 C30 C35:C37 C39:C41">
-      <formula1>$B$45:$B$48</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="B10 B13 B16 B18 B22 B25 B28 B30 B35:B36 B39 B42:B44 B46">
+      <formula1>$C$51:$C$54</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B10 B13 B16 B18 B22 B25 B28 B30 B35:B37 B39:B41">
-      <formula1>$C$45:$C$48</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="C10 C13 C16 C18 C22 C25 C28 C30 C35:C36 C39 C42:C44 C46">
+      <formula1>$B$51:$B$54</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="H46"/>
+    <hyperlink r:id="rId2" ref="I46"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>